<commit_message>
Changed pdf to docx
</commit_message>
<xml_diff>
--- a/documents/PRESS_RELEASE_CLIPPING.xlsx
+++ b/documents/PRESS_RELEASE_CLIPPING.xlsx
@@ -437,7 +437,7 @@
     <t>Socrates project</t>
   </si>
   <si>
-    <t>https://www.esleondiario.com/2018/11/07/como-detectar-y-detener-a-los-saboteadores-del-espectro/</t>
+    <t>dasd</t>
   </si>
   <si>
     <t>Number of Posts</t>
@@ -2904,7 +2904,7 @@
         <v>156</v>
       </c>
       <c r="L3" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="M3" t="s">
         <v>157</v>

</xml_diff>

<commit_message>
Added Dissemination sheet to excel
</commit_message>
<xml_diff>
--- a/documents/PRESS_RELEASE_CLIPPING.xlsx
+++ b/documents/PRESS_RELEASE_CLIPPING.xlsx
@@ -6,16 +6,14 @@
   <sheets>
     <sheet sheetId="1" name="Clipping" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="SM Shares" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Dissemination Data" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="158">
-  <si>
-    <t>Audience</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="181">
   <si>
     <t>Month</t>
   </si>
@@ -83,6 +81,9 @@
     <t>Original URL</t>
   </si>
   <si>
+    <t>Other Media Impact</t>
+  </si>
+  <si>
     <t>Por Azar</t>
   </si>
   <si>
@@ -486,6 +487,75 @@
   </si>
   <si>
     <t>https://www.networks.imdea.org/whats-new/news/2017/ralf-steinmetz-appointed-first-itg-fellow-vde-german-association-electrical</t>
+  </si>
+  <si>
+    <t>Lead Paragraph</t>
+  </si>
+  <si>
+    <t>PR/NEWS</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Other Media Dissemination</t>
+  </si>
+  <si>
+    <t>Vía libre para el uso de ondas milimétricas con la tecnología  5G</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet consectetur adipisicing elit. Dignissimos, quaerat deleniti? Quaerat dolor fugiat provident aperiam vitae odit perspiciatis nemo consequuntur tempora consequatur facere architecto, molestias obcaecati id iusto voluptas!</t>
+  </si>
+  <si>
+    <t>https://www.networks.imdea.org/es/printpdf/7220</t>
+  </si>
+  <si>
+    <t>Investigadores de la UC3M e IMDEA Networks presentan sus novedades sobre 5G en el Mobile World Congress 2018</t>
+  </si>
+  <si>
+    <t>https://www.networks.imdea.org/es/printpdf/7289</t>
+  </si>
+  <si>
+    <t>Procesamiento dinámico en redes 5G</t>
+  </si>
+  <si>
+    <t>https://www.networks.imdea.org/es/actualidad/noticias/2018/procesamiento-dinamico-redes-5g</t>
+  </si>
+  <si>
+    <t>IMDEA Networks participa en el primer máster sobre 5G del mundo</t>
+  </si>
+  <si>
+    <t>https://www.networks.imdea.org/es/actualidad/noticias/2018/imdea-networks-participa-primer-master-sobre-5g-mundo</t>
+  </si>
+  <si>
+    <t>https://www.networks.imdea.org/es/printpdf/7274</t>
+  </si>
+  <si>
+    <t>Miles de aplicaciones móviles para niños pueden estar violando su privacidad</t>
+  </si>
+  <si>
+    <t>https://www.networks.imdea.org/es/printpdf/7357</t>
+  </si>
+  <si>
+    <t>Detectar y detener a los saboteadores del espectro</t>
+  </si>
+  <si>
+    <t>https://www.networks.imdea.org/es/printpdf/7573</t>
+  </si>
+  <si>
+    <t>Desarrollan una solución de red de transporte flexible y dinámica para las comunicaciones 5G</t>
+  </si>
+  <si>
+    <t>https://www.networks.imdea.org/es/printpdf/7405</t>
+  </si>
+  <si>
+    <t>Desarrollan una herramienta que muestra la brecha de género en Facebook</t>
+  </si>
+  <si>
+    <t>https://www.networks.imdea.org/es/actualidad/noticias/2018/desarrollan-una-herramienta-que-muestra-brecha-genero-facebook</t>
+  </si>
+  <si>
+    <t>https://www.networks.imdea.org/es/actualidad/noticias/2018/un-sistema-posicionamiento-impulsa-futura-innovacion-inalambrica</t>
   </si>
 </sst>
 </file>
@@ -948,1825 +1018,1825 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="2">
         <v>43102</v>
       </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
         <v>31</v>
       </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
       <c r="M2" t="b">
         <v>0</v>
       </c>
-      <c r="N2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2" t="b">
-        <v>1</v>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" t="s">
         <v>33</v>
       </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
       <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>34</v>
       </c>
       <c r="U2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V2" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" t="s">
         <v>36</v>
+      </c>
+      <c r="W2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="2">
         <v>43103.04166666667</v>
       </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
         <v>31</v>
       </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
+      <c r="L3" t="b">
+        <v>0</v>
       </c>
       <c r="M3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" t="b">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" t="s">
         <v>39</v>
       </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
       <c r="S3" t="b">
-        <v>1</v>
-      </c>
-      <c r="T3" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>34</v>
       </c>
       <c r="U3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V3" t="s">
-        <v>35</v>
-      </c>
-      <c r="W3" t="s">
         <v>40</v>
+      </c>
+      <c r="W3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="2">
         <v>43103.04166666667</v>
       </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" t="s">
         <v>31</v>
       </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
       <c r="M4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" t="b">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>32</v>
       </c>
       <c r="Q4" t="s">
-        <v>32</v>
-      </c>
-      <c r="R4" t="s">
         <v>39</v>
       </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
       <c r="S4" t="b">
-        <v>1</v>
-      </c>
-      <c r="T4" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
+        <v>34</v>
       </c>
       <c r="U4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V4" t="s">
-        <v>35</v>
-      </c>
-      <c r="W4" t="s">
         <v>45</v>
+      </c>
+      <c r="W4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="2">
         <v>43117.04166666667</v>
       </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" t="s">
         <v>49</v>
       </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
       <c r="M5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
         <v>39</v>
       </c>
+      <c r="R5" t="b">
+        <v>1</v>
+      </c>
       <c r="S5" t="b">
-        <v>1</v>
-      </c>
-      <c r="T5" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
+        <v>34</v>
       </c>
       <c r="U5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V5" t="s">
-        <v>35</v>
-      </c>
-      <c r="W5" t="s">
         <v>50</v>
+      </c>
+      <c r="W5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="B6" s="2">
         <v>43158.04166666667</v>
       </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="K6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" t="s">
         <v>31</v>
       </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
       <c r="M6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
         <v>39</v>
       </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
       <c r="S6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>34</v>
       </c>
       <c r="U6" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="V6" t="s">
-        <v>55</v>
-      </c>
-      <c r="W6" t="s">
         <v>56</v>
+      </c>
+      <c r="W6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" s="2">
+      <c r="B7" s="2">
         <v>43158.04166666667</v>
       </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="K7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" t="s">
         <v>49</v>
       </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
       <c r="M7" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" t="b">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>60</v>
       </c>
       <c r="Q7" t="s">
-        <v>60</v>
-      </c>
-      <c r="R7" t="s">
         <v>39</v>
       </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
       <c r="S7" t="b">
-        <v>1</v>
-      </c>
-      <c r="T7" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
+        <v>34</v>
       </c>
       <c r="U7" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="V7" t="s">
-        <v>55</v>
-      </c>
-      <c r="W7" t="s">
         <v>61</v>
+      </c>
+      <c r="W7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="B8" s="2">
         <v>43169.04166666667</v>
       </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" t="s">
         <v>31</v>
       </c>
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
       <c r="M8" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" t="b">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>60</v>
       </c>
       <c r="Q8" t="s">
-        <v>60</v>
-      </c>
-      <c r="R8" t="s">
         <v>39</v>
       </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
       <c r="S8" t="b">
-        <v>1</v>
-      </c>
-      <c r="T8" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T8" t="s">
+        <v>65</v>
       </c>
       <c r="U8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V8" t="s">
-        <v>66</v>
-      </c>
-      <c r="W8" t="s">
         <v>67</v>
+      </c>
+      <c r="W8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="B9" s="2">
         <v>43170.04166666667</v>
       </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="J9" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="K9" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" t="s">
         <v>31</v>
       </c>
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
       <c r="M9" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>60</v>
       </c>
       <c r="Q9" t="s">
-        <v>60</v>
-      </c>
-      <c r="R9" t="s">
         <v>39</v>
       </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
       <c r="S9" t="b">
-        <v>1</v>
-      </c>
-      <c r="T9" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
+        <v>65</v>
       </c>
       <c r="U9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V9" t="s">
-        <v>66</v>
-      </c>
-      <c r="W9" t="s">
         <v>71</v>
+      </c>
+      <c r="W9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="2">
+      <c r="B10" s="2">
         <v>43171</v>
       </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" t="s">
         <v>31</v>
       </c>
-      <c r="J10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" t="s">
-        <v>31</v>
+      <c r="L10" t="b">
+        <v>0</v>
       </c>
       <c r="M10" t="b">
         <v>0</v>
       </c>
-      <c r="N10" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" t="b">
-        <v>1</v>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>36</v>
       </c>
       <c r="Q10" t="s">
-        <v>36</v>
-      </c>
-      <c r="R10" t="s">
         <v>33</v>
       </c>
+      <c r="R10" t="b">
+        <v>1</v>
+      </c>
       <c r="S10" t="b">
-        <v>1</v>
-      </c>
-      <c r="T10" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>65</v>
       </c>
       <c r="U10" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="V10" t="s">
-        <v>75</v>
-      </c>
-      <c r="W10" t="s">
         <v>76</v>
+      </c>
+      <c r="W10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="2">
+      <c r="B11" s="2">
         <v>43171.04166666667</v>
       </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I11" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="J11" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="K11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" t="s">
         <v>49</v>
       </c>
+      <c r="L11" t="b">
+        <v>0</v>
+      </c>
       <c r="M11" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11" t="b">
-        <v>1</v>
-      </c>
-      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
         <v>39</v>
       </c>
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
       <c r="S11" t="b">
-        <v>1</v>
-      </c>
-      <c r="T11" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>65</v>
       </c>
       <c r="U11" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="V11" t="s">
-        <v>75</v>
-      </c>
-      <c r="W11" t="s">
         <v>78</v>
+      </c>
+      <c r="W11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12" s="2">
+      <c r="B12" s="2">
         <v>43173.04166666667</v>
       </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="I12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J12" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" t="s">
         <v>49</v>
       </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
       <c r="M12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12" t="b">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>60</v>
       </c>
       <c r="Q12" t="s">
-        <v>60</v>
-      </c>
-      <c r="R12" t="s">
         <v>39</v>
       </c>
+      <c r="R12" t="b">
+        <v>1</v>
+      </c>
       <c r="S12" t="b">
-        <v>1</v>
-      </c>
-      <c r="T12" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>65</v>
       </c>
       <c r="U12" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="V12" t="s">
-        <v>75</v>
-      </c>
-      <c r="W12" t="s">
         <v>81</v>
+      </c>
+      <c r="W12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13" s="2">
+      <c r="B13" s="2">
         <v>43175.04166666667</v>
       </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I13" t="s">
+        <v>77</v>
+      </c>
+      <c r="J13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" t="s">
         <v>31</v>
       </c>
-      <c r="J13" t="s">
-        <v>77</v>
-      </c>
-      <c r="K13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" t="s">
-        <v>31</v>
+      <c r="L13" t="b">
+        <v>0</v>
       </c>
       <c r="M13" t="b">
-        <v>0</v>
-      </c>
-      <c r="N13" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13" t="b">
-        <v>1</v>
-      </c>
-      <c r="R13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
         <v>39</v>
       </c>
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
       <c r="S13" t="b">
-        <v>1</v>
-      </c>
-      <c r="T13" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>65</v>
       </c>
       <c r="U13" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="V13" t="s">
-        <v>75</v>
-      </c>
-      <c r="W13" t="s">
         <v>84</v>
+      </c>
+      <c r="W13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
         <v>4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="B14" s="2">
         <v>43210.08333333333</v>
       </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I14" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" t="s">
         <v>31</v>
       </c>
-      <c r="J14" t="s">
-        <v>85</v>
-      </c>
-      <c r="K14" t="s">
-        <v>30</v>
-      </c>
-      <c r="L14" t="s">
-        <v>31</v>
+      <c r="L14" t="b">
+        <v>0</v>
       </c>
       <c r="M14" t="b">
-        <v>0</v>
-      </c>
-      <c r="N14" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P14" t="s">
+        <v>86</v>
       </c>
       <c r="Q14" t="s">
-        <v>86</v>
-      </c>
-      <c r="R14" t="s">
         <v>39</v>
       </c>
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
       <c r="S14" t="b">
-        <v>1</v>
-      </c>
-      <c r="T14" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>34</v>
       </c>
       <c r="U14" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="V14" t="s">
-        <v>87</v>
-      </c>
-      <c r="W14" t="s">
         <v>88</v>
+      </c>
+      <c r="W14" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
         <v>4</v>
       </c>
-      <c r="C15" s="2">
+      <c r="B15" s="2">
         <v>43212.08333333333</v>
       </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="I15" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="K15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L15" t="s">
         <v>31</v>
       </c>
+      <c r="L15" t="b">
+        <v>0</v>
+      </c>
       <c r="M15" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" t="b">
-        <v>1</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="b">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>86</v>
       </c>
       <c r="Q15" t="s">
-        <v>86</v>
-      </c>
-      <c r="R15" t="s">
         <v>39</v>
       </c>
+      <c r="R15" t="b">
+        <v>1</v>
+      </c>
       <c r="S15" t="b">
-        <v>1</v>
-      </c>
-      <c r="T15" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>34</v>
       </c>
       <c r="U15" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="V15" t="s">
-        <v>87</v>
-      </c>
-      <c r="W15" t="s">
         <v>89</v>
+      </c>
+      <c r="W15" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
         <v>4</v>
       </c>
-      <c r="C16" s="2">
+      <c r="B16" s="2">
         <v>43213.08333333333</v>
       </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I16" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="J16" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>30</v>
-      </c>
-      <c r="L16" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="L16" t="b">
+        <v>0</v>
       </c>
       <c r="M16" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" t="b">
-        <v>1</v>
-      </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
-      <c r="P16" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16" t="b">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>86</v>
       </c>
       <c r="Q16" t="s">
-        <v>86</v>
-      </c>
-      <c r="R16" t="s">
         <v>39</v>
       </c>
+      <c r="R16" t="b">
+        <v>1</v>
+      </c>
       <c r="S16" t="b">
-        <v>1</v>
-      </c>
-      <c r="T16" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T16" t="s">
+        <v>34</v>
       </c>
       <c r="U16" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="V16" t="s">
-        <v>87</v>
-      </c>
-      <c r="W16" t="s">
         <v>92</v>
+      </c>
+      <c r="W16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17">
         <v>4</v>
       </c>
-      <c r="C17" s="2">
+      <c r="B17" s="2">
         <v>43215.08333333333</v>
       </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="I17" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="J17" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" t="s">
         <v>49</v>
       </c>
+      <c r="L17" t="b">
+        <v>0</v>
+      </c>
       <c r="M17" t="b">
-        <v>0</v>
-      </c>
-      <c r="N17" t="b">
-        <v>1</v>
-      </c>
-      <c r="O17">
-        <v>1</v>
-      </c>
-      <c r="P17" t="b">
-        <v>1</v>
-      </c>
-      <c r="R17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
         <v>39</v>
       </c>
+      <c r="R17" t="b">
+        <v>1</v>
+      </c>
       <c r="S17" t="b">
-        <v>1</v>
-      </c>
-      <c r="T17" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T17" t="s">
+        <v>34</v>
       </c>
       <c r="U17" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="V17" t="s">
-        <v>96</v>
-      </c>
-      <c r="W17" t="s">
         <v>97</v>
+      </c>
+      <c r="W17" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
         <v>5</v>
       </c>
-      <c r="C18" s="2">
+      <c r="B18" s="2">
         <v>43224</v>
       </c>
+      <c r="C18" t="s">
+        <v>98</v>
+      </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H18" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="I18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J18" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="K18" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18" t="s">
         <v>49</v>
       </c>
+      <c r="L18" t="b">
+        <v>0</v>
+      </c>
       <c r="M18" t="b">
-        <v>0</v>
-      </c>
-      <c r="N18" t="b">
-        <v>1</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18" t="b">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>102</v>
       </c>
       <c r="Q18" t="s">
-        <v>102</v>
-      </c>
-      <c r="R18" t="s">
         <v>33</v>
       </c>
+      <c r="R18" t="b">
+        <v>1</v>
+      </c>
       <c r="S18" t="b">
-        <v>1</v>
-      </c>
-      <c r="T18" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T18" t="s">
+        <v>34</v>
       </c>
       <c r="U18" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="V18" t="s">
-        <v>96</v>
-      </c>
-      <c r="W18" t="s">
         <v>103</v>
+      </c>
+      <c r="W18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19">
         <v>5</v>
       </c>
-      <c r="C19" s="2">
+      <c r="B19" s="2">
         <v>43250</v>
       </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I19" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="J19" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="K19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L19" t="s">
         <v>31</v>
       </c>
+      <c r="L19" t="b">
+        <v>0</v>
+      </c>
       <c r="M19" t="b">
         <v>0</v>
       </c>
-      <c r="N19" t="b">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19" t="b">
-        <v>1</v>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>36</v>
       </c>
       <c r="Q19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R19" t="s">
         <v>39</v>
       </c>
+      <c r="R19" t="b">
+        <v>1</v>
+      </c>
       <c r="S19" t="b">
-        <v>1</v>
-      </c>
-      <c r="T19" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T19" t="s">
+        <v>34</v>
       </c>
       <c r="U19" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="V19" t="s">
-        <v>107</v>
-      </c>
-      <c r="W19" t="s">
         <v>108</v>
+      </c>
+      <c r="W19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20">
         <v>6</v>
       </c>
-      <c r="C20" s="2">
+      <c r="B20" s="2">
         <v>43252.08333333333</v>
       </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="I20" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="J20" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="K20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L20" t="s">
         <v>31</v>
       </c>
+      <c r="L20" t="b">
+        <v>0</v>
+      </c>
       <c r="M20" t="b">
-        <v>0</v>
-      </c>
-      <c r="N20" t="b">
-        <v>1</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="P20" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20" t="b">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>60</v>
       </c>
       <c r="Q20" t="s">
-        <v>60</v>
-      </c>
-      <c r="R20" t="s">
         <v>39</v>
       </c>
+      <c r="R20" t="b">
+        <v>1</v>
+      </c>
       <c r="S20" t="b">
-        <v>1</v>
-      </c>
-      <c r="T20" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T20" t="s">
+        <v>34</v>
       </c>
       <c r="U20" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="V20" t="s">
-        <v>107</v>
-      </c>
-      <c r="W20" t="s">
         <v>112</v>
+      </c>
+      <c r="W20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
         <v>6</v>
       </c>
-      <c r="C21" s="2">
+      <c r="B21" s="2">
         <v>43271.08333333333</v>
       </c>
+      <c r="C21" t="s">
+        <v>113</v>
+      </c>
       <c r="D21" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E21" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H21" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="I21" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="J21" t="s">
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="K21" t="s">
-        <v>30</v>
-      </c>
-      <c r="L21" t="s">
         <v>31</v>
       </c>
+      <c r="L21" t="b">
+        <v>0</v>
+      </c>
       <c r="M21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21" t="b">
-        <v>1</v>
-      </c>
-      <c r="R21" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="s">
         <v>33</v>
       </c>
+      <c r="R21" t="b">
+        <v>1</v>
+      </c>
       <c r="S21" t="b">
-        <v>1</v>
-      </c>
-      <c r="T21" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T21" t="s">
+        <v>65</v>
       </c>
       <c r="U21" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="V21" t="s">
-        <v>116</v>
-      </c>
-      <c r="W21" t="s">
         <v>117</v>
+      </c>
+      <c r="W21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
         <v>6</v>
       </c>
-      <c r="C22" s="2">
+      <c r="B22" s="2">
         <v>43271.08333333333</v>
       </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H22" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="I22" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="J22" t="s">
-        <v>118</v>
+        <v>30</v>
       </c>
       <c r="K22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L22" t="s">
         <v>31</v>
       </c>
+      <c r="L22" t="b">
+        <v>0</v>
+      </c>
       <c r="M22" t="b">
-        <v>0</v>
-      </c>
-      <c r="N22" t="b">
-        <v>1</v>
-      </c>
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="P22" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22" t="b">
+        <v>1</v>
+      </c>
+      <c r="P22" t="s">
+        <v>119</v>
       </c>
       <c r="Q22" t="s">
-        <v>119</v>
-      </c>
-      <c r="R22" t="s">
         <v>39</v>
       </c>
+      <c r="R22" t="b">
+        <v>1</v>
+      </c>
       <c r="S22" t="b">
-        <v>1</v>
-      </c>
-      <c r="T22" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T22" t="s">
+        <v>65</v>
       </c>
       <c r="U22" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="V22" t="s">
-        <v>116</v>
-      </c>
-      <c r="W22" t="s">
         <v>120</v>
+      </c>
+      <c r="W22" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23">
         <v>6</v>
       </c>
-      <c r="C23" s="2">
+      <c r="B23" s="2">
         <v>43271.08333333333</v>
       </c>
+      <c r="C23" t="s">
+        <v>121</v>
+      </c>
       <c r="D23" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E23" t="s">
-        <v>122</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H23" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="I23" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="J23" t="s">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="K23" t="s">
-        <v>30</v>
-      </c>
-      <c r="L23" t="s">
         <v>31</v>
       </c>
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
       <c r="M23" t="b">
-        <v>0</v>
-      </c>
-      <c r="N23" t="b">
-        <v>1</v>
-      </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23" t="b">
+        <v>1</v>
+      </c>
+      <c r="P23" t="s">
+        <v>119</v>
       </c>
       <c r="Q23" t="s">
-        <v>119</v>
-      </c>
-      <c r="R23" t="s">
         <v>39</v>
       </c>
+      <c r="R23" t="b">
+        <v>1</v>
+      </c>
       <c r="S23" t="b">
-        <v>1</v>
-      </c>
-      <c r="T23" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T23" t="s">
+        <v>65</v>
       </c>
       <c r="U23" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="V23" t="s">
-        <v>116</v>
-      </c>
-      <c r="W23" t="s">
         <v>124</v>
+      </c>
+      <c r="W23" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24">
         <v>6</v>
       </c>
-      <c r="C24" s="2">
+      <c r="B24" s="2">
         <v>43271.08333333333</v>
       </c>
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E24" t="s">
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I24" t="s">
-        <v>28</v>
+        <v>125</v>
       </c>
       <c r="J24" t="s">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="K24" t="s">
-        <v>30</v>
-      </c>
-      <c r="L24" t="s">
         <v>31</v>
       </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
       <c r="M24" t="b">
-        <v>0</v>
-      </c>
-      <c r="N24" t="b">
-        <v>1</v>
-      </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-      <c r="P24" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" t="s">
+        <v>119</v>
       </c>
       <c r="Q24" t="s">
-        <v>119</v>
-      </c>
-      <c r="R24" t="s">
         <v>33</v>
       </c>
+      <c r="R24" t="b">
+        <v>1</v>
+      </c>
       <c r="S24" t="b">
-        <v>1</v>
-      </c>
-      <c r="T24" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T24" t="s">
+        <v>65</v>
       </c>
       <c r="U24" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="V24" t="s">
-        <v>116</v>
-      </c>
-      <c r="W24" t="s">
         <v>126</v>
+      </c>
+      <c r="W24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25">
         <v>6</v>
       </c>
-      <c r="C25" s="2">
+      <c r="B25" s="2">
         <v>43271.08333333333</v>
       </c>
+      <c r="C25" t="s">
+        <v>127</v>
+      </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E25" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="I25" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>30</v>
       </c>
       <c r="K25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L25" t="s">
         <v>31</v>
       </c>
+      <c r="L25" t="b">
+        <v>0</v>
+      </c>
       <c r="M25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N25" t="b">
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25" t="b">
+        <v>1</v>
+      </c>
+      <c r="P25" t="s">
+        <v>130</v>
       </c>
       <c r="Q25" t="s">
-        <v>130</v>
-      </c>
-      <c r="R25" t="s">
         <v>39</v>
       </c>
+      <c r="R25" t="b">
+        <v>1</v>
+      </c>
       <c r="S25" t="b">
-        <v>1</v>
-      </c>
-      <c r="T25" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T25" t="s">
+        <v>65</v>
       </c>
       <c r="U25" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="V25" t="s">
-        <v>116</v>
-      </c>
-      <c r="W25" t="s">
         <v>131</v>
+      </c>
+      <c r="W25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26">
         <v>9</v>
       </c>
-      <c r="C26" s="2">
+      <c r="B26" s="2">
         <v>43347.08333333333</v>
       </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H26" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I26" t="s">
+        <v>132</v>
+      </c>
+      <c r="J26" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" t="s">
         <v>31</v>
       </c>
-      <c r="J26" t="s">
-        <v>132</v>
-      </c>
-      <c r="K26" t="s">
-        <v>30</v>
-      </c>
-      <c r="L26" t="s">
-        <v>31</v>
+      <c r="L26" t="b">
+        <v>0</v>
       </c>
       <c r="M26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N26" t="b">
-        <v>1</v>
-      </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26" t="b">
-        <v>1</v>
-      </c>
-      <c r="R26" t="s">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="s">
         <v>39</v>
       </c>
+      <c r="R26" t="b">
+        <v>1</v>
+      </c>
       <c r="S26" t="b">
-        <v>1</v>
-      </c>
-      <c r="T26" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T26" t="s">
+        <v>65</v>
       </c>
       <c r="U26" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="V26" t="s">
-        <v>133</v>
-      </c>
-      <c r="W26" t="s">
         <v>134</v>
+      </c>
+      <c r="W26" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27">
         <v>11</v>
       </c>
-      <c r="C27" s="2">
+      <c r="B27" s="2">
         <v>43411</v>
       </c>
+      <c r="C27" t="s">
+        <v>135</v>
+      </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
       <c r="H27" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
       <c r="I27" t="s">
-        <v>28</v>
+        <v>138</v>
       </c>
       <c r="J27" t="s">
-        <v>138</v>
+        <v>30</v>
       </c>
       <c r="K27" t="s">
-        <v>30</v>
-      </c>
-      <c r="L27" t="s">
         <v>31</v>
       </c>
+      <c r="L27" t="b">
+        <v>1</v>
+      </c>
       <c r="M27" t="b">
         <v>1</v>
       </c>
-      <c r="N27" t="b">
-        <v>1</v>
-      </c>
-      <c r="O27">
-        <v>1</v>
-      </c>
-      <c r="P27" t="b">
-        <v>1</v>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27" t="b">
+        <v>1</v>
+      </c>
+      <c r="P27" t="s">
+        <v>139</v>
       </c>
       <c r="Q27" t="s">
-        <v>139</v>
-      </c>
-      <c r="R27" t="s">
         <v>39</v>
       </c>
+      <c r="R27" t="b">
+        <v>1</v>
+      </c>
       <c r="S27" t="b">
-        <v>1</v>
-      </c>
-      <c r="T27" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T27" t="s">
+        <v>34</v>
       </c>
       <c r="U27" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="V27" t="s">
-        <v>140</v>
-      </c>
-      <c r="W27" t="s">
         <v>141</v>
+      </c>
+      <c r="W27" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2786,13 +2856,13 @@
         <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>143</v>
@@ -2801,22 +2871,22 @@
         <v>144</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>145</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>146</v>
@@ -2914,7 +2984,305 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1"/>
+  <autoFilter ref="A1:V1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43098.04166666667</v>
+      </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43098.04166666667</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43165.04166666667</v>
+      </c>
+      <c r="C4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43172.04166666667</v>
+      </c>
+      <c r="C5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43209.08333333333</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43214.08333333333</v>
+      </c>
+      <c r="C7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43231.08333333333</v>
+      </c>
+      <c r="C8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>175</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>43250.08333333333</v>
+      </c>
+      <c r="C9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43271.08333333333</v>
+      </c>
+      <c r="C10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>43343.08333333333</v>
+      </c>
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" t="s">
+        <v>180</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Separated report by months
</commit_message>
<xml_diff>
--- a/documents/PRESS_RELEASE_CLIPPING.xlsx
+++ b/documents/PRESS_RELEASE_CLIPPING.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="166">
   <si>
     <t>Month</t>
   </si>
@@ -123,123 +123,126 @@
     <t>mm waves and 5G technology</t>
   </si>
   <si>
+    <t>https://www.porazar.com/news/via-libre-para-el-uso-de-ondas-milimetricas-con-la-tecnologia-5g/</t>
+  </si>
+  <si>
+    <t>Radhames DecaNo</t>
+  </si>
+  <si>
+    <t>http://www.radhamesdecaNo.com</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>Specialised</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>http://www.radhamesdecano.com/wp/ciencia/fisica/via-libre-uso-de-ondas-milimetricas-para-5g/</t>
+  </si>
+  <si>
+    <t>Candas 365</t>
+  </si>
+  <si>
+    <t>https://candas365.es</t>
+  </si>
+  <si>
+    <t>https://candas365.es/noticias/via-libre-para-el-uso-de-ondas-milimetricas-con-la-tecnologia-5g/</t>
+  </si>
+  <si>
+    <t>Telebosco</t>
+  </si>
+  <si>
+    <t>www.telecobosco.com</t>
+  </si>
+  <si>
+    <t>Institutional</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>http://telecobosco.com/via-libre-uso-ondas-milimetricas-la-tecnologia-5g/</t>
+  </si>
+  <si>
+    <t>Leganews</t>
+  </si>
+  <si>
+    <t>https://www.leganews.es/</t>
+  </si>
+  <si>
+    <t>Investigadores de la UC3M presentan sus Novedades sobre 5G en el Mobile World Congress 2018</t>
+  </si>
+  <si>
+    <t>Arturo Azcorra, Director of IMDEA Networks, Telematics professor at UC3M and Vice President of 5TONIC</t>
+  </si>
+  <si>
+    <t>IMDEA Networks and UC3M at MWC 2018</t>
+  </si>
+  <si>
+    <t>https://www.leganews.es/5g-uc3m-imdea-mobile-world-congress/</t>
+  </si>
+  <si>
+    <t>Nuevo Crónica</t>
+  </si>
+  <si>
+    <t>https://nuevocronica.es/</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Investigadores de la UC3M e IMDEA Networks presentan sus Novedades sobre 5G en el Mobile World Congress 2018</t>
+  </si>
+  <si>
+    <t>https://nuevocronica.es/investigadores-de-la-uc3m-e-imdea-networks-presentan-sus-novedades-sobre-5g-en-el-mobile-world-congress-2018-42701</t>
+  </si>
+  <si>
+    <t>Polemica Guanajuato</t>
+  </si>
+  <si>
+    <t>https://www.polemicaguanajuato.com</t>
+  </si>
+  <si>
+    <t>Una investigación busca lograr un procesamiento dinámico y de alto rendimiento del tráfico de redes 5G</t>
+  </si>
+  <si>
+    <t>NEWS</t>
+  </si>
+  <si>
+    <t>Industrial PhD-Telcaria</t>
+  </si>
+  <si>
+    <t>http://polemicaguanajuato.com/una-investigacion-busca-lograr-un-procesamiento-dinamico-y-de-alto-rendimiento-del-trafico-en-redes-5g/</t>
+  </si>
+  <si>
+    <t>Salamanca 24H</t>
+  </si>
+  <si>
+    <t>https://www.salamanca24horas.com</t>
+  </si>
+  <si>
+    <t>Una investigación busca lograr un procesamiento dinámico y de alto rendimiento del tráfico en redes 5G</t>
+  </si>
+  <si>
+    <t>https://www.salamanca24horas.com/texto-diario/mostrar/1026619/investigacion-busca-lograr-procesamiento-dinamico-alto-rendimiento-trafico-redes-5g</t>
+  </si>
+  <si>
+    <t>Diario Vasco</t>
+  </si>
+  <si>
+    <t>https://www.diariovasco.com</t>
+  </si>
+  <si>
+    <t>Universidad Carlos III y Ericsson presentan primer máster sobre 5G de España</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Candas 365</t>
-  </si>
-  <si>
-    <t>https://candas365.es</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>https://candas365.es/noticias/via-libre-para-el-uso-de-ondas-milimetricas-con-la-tecnologia-5g/</t>
-  </si>
-  <si>
-    <t>Radhames DecaNo</t>
-  </si>
-  <si>
-    <t>http://www.radhamesdecaNo.com</t>
-  </si>
-  <si>
-    <t>Blog</t>
-  </si>
-  <si>
-    <t>Specialised</t>
-  </si>
-  <si>
-    <t>http://www.radhamesdecano.com/wp/ciencia/fisica/via-libre-uso-de-ondas-milimetricas-para-5g/</t>
-  </si>
-  <si>
-    <t>Telebosco</t>
-  </si>
-  <si>
-    <t>www.telecobosco.com</t>
-  </si>
-  <si>
-    <t>Institutional</t>
-  </si>
-  <si>
-    <t>Article</t>
-  </si>
-  <si>
-    <t>http://telecobosco.com/via-libre-uso-ondas-milimetricas-la-tecnologia-5g/</t>
-  </si>
-  <si>
-    <t>Nuevo Crónica</t>
-  </si>
-  <si>
-    <t>https://nuevocronica.es/</t>
-  </si>
-  <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>Investigadores de la UC3M e IMDEA Networks presentan sus Novedades sobre 5G en el Mobile World Congress 2018</t>
-  </si>
-  <si>
-    <t>IMDEA Networks and UC3M at MWC 2018</t>
-  </si>
-  <si>
-    <t>https://nuevocronica.es/investigadores-de-la-uc3m-e-imdea-networks-presentan-sus-novedades-sobre-5g-en-el-mobile-world-congress-2018-42701</t>
-  </si>
-  <si>
-    <t>Leganews</t>
-  </si>
-  <si>
-    <t>https://www.leganews.es/</t>
-  </si>
-  <si>
-    <t>Investigadores de la UC3M presentan sus Novedades sobre 5G en el Mobile World Congress 2018</t>
-  </si>
-  <si>
-    <t>Arturo Azcorra, Director of IMDEA Networks, Telematics professor at UC3M and Vice President of 5TONIC</t>
-  </si>
-  <si>
-    <t>https://www.leganews.es/5g-uc3m-imdea-mobile-world-congress/</t>
-  </si>
-  <si>
-    <t>Polemica Guanajuato</t>
-  </si>
-  <si>
-    <t>https://www.polemicaguanajuato.com</t>
-  </si>
-  <si>
-    <t>Una investigación busca lograr un procesamiento dinámico y de alto rendimiento del tráfico de redes 5G</t>
-  </si>
-  <si>
-    <t>NEWS</t>
-  </si>
-  <si>
-    <t>Industrial PhD-Telcaria</t>
-  </si>
-  <si>
-    <t>http://polemicaguanajuato.com/una-investigacion-busca-lograr-un-procesamiento-dinamico-y-de-alto-rendimiento-del-trafico-en-redes-5g/</t>
-  </si>
-  <si>
-    <t>Salamanca 24H</t>
-  </si>
-  <si>
-    <t>https://www.salamanca24horas.com</t>
-  </si>
-  <si>
-    <t>Una investigación busca lograr un procesamiento dinámico y de alto rendimiento del tráfico en redes 5G</t>
-  </si>
-  <si>
-    <t>https://www.salamanca24horas.com/texto-diario/mostrar/1026619/investigacion-busca-lograr-procesamiento-dinamico-alto-rendimiento-trafico-redes-5g</t>
-  </si>
-  <si>
-    <t>Diario Vasco</t>
-  </si>
-  <si>
-    <t>https://www.diariovasco.com</t>
-  </si>
-  <si>
-    <t>Universidad Carlos III y Ericsson presentan primer máster sobre 5G de España</t>
-  </si>
-  <si>
     <t>First 5G master's degree</t>
   </si>
   <si>
@@ -354,6 +357,24 @@
     <t>https://www.catalunyavanguardista.com/red-de-transporte-5g-integrada/</t>
   </si>
   <si>
+    <t>Madrid Actual</t>
+  </si>
+  <si>
+    <t>https://www.madridactual.es/</t>
+  </si>
+  <si>
+    <t>La Carlos III desarrolla una herramienta para medir la brecha de género en Facebook</t>
+  </si>
+  <si>
+    <t>David García, del CHS y la Universidad Médica de Viena</t>
+  </si>
+  <si>
+    <t>Facebook gender divide</t>
+  </si>
+  <si>
+    <t>https://www.madridactual.es/201806207673897/la-carlos-iii-desarrolla-una-herramienta-para-medir-la-brecha-de-genero-en-facebook</t>
+  </si>
+  <si>
     <t>MadridPress</t>
   </si>
   <si>
@@ -363,18 +384,21 @@
     <t>Las desigualdades en el uso de Facebook son un reflejo de la brecha de género en otros ámbitos</t>
   </si>
   <si>
-    <t>Facebook gender divide</t>
-  </si>
-  <si>
     <t>https://madridpress.com/not/240728/las-desigualdades-en-el-uso-de-facebook-son-un-reflejo-de-la-brecha-de-genero-en-otros-ambitos/</t>
   </si>
   <si>
+    <t>Las mujeres usan más Facebook que los hombres</t>
+  </si>
+  <si>
+    <t>David García, del CHS y la Universidad Médica de Viena, Esteban Moro , profesor de matemáticas de la UC3M y profesor visitante en el MIT Media Lab, Rubén Cuevas, departamento Ingeniería Telemática UC3M</t>
+  </si>
+  <si>
+    <t>https://www.catalunyavanguardista.com/las-mujeres-usan-mas-facebook-que-los-hombres/</t>
+  </si>
+  <si>
     <t>Nueva herramienta que muestra la brecha de género en Facebook</t>
   </si>
   <si>
-    <t>David García, del CHS y la Universidad Médica de Viena, Esteban Moro , profesor de matemáticas de la UC3M y profesor visitante en el MIT Media Lab, Rubén Cuevas, departamento Ingeniería Telemática UC3M</t>
-  </si>
-  <si>
     <t>https://www.leganews.es/nueva-herramienta-que-muestra-la-brecha-de-genero-en-facebook/</t>
   </si>
   <si>
@@ -390,27 +414,6 @@
     <t>https://andaluciagame.andaluciainformacion.es/tecnologia/crean-una-herramienta-que-muestra-la-brecha-de-genero-en-facebook/</t>
   </si>
   <si>
-    <t>Las mujeres usan más Facebook que los hombres</t>
-  </si>
-  <si>
-    <t>https://www.catalunyavanguardista.com/las-mujeres-usan-mas-facebook-que-los-hombres/</t>
-  </si>
-  <si>
-    <t>Madrid Actual</t>
-  </si>
-  <si>
-    <t>https://www.madridactual.es/</t>
-  </si>
-  <si>
-    <t>La Carlos III desarrolla una herramienta para medir la brecha de género en Facebook</t>
-  </si>
-  <si>
-    <t>David García, del CHS y la Universidad Médica de Viena</t>
-  </si>
-  <si>
-    <t>https://www.madridactual.es/201806207673897/la-carlos-iii-desarrolla-una-herramienta-para-medir-la-brecha-de-genero-en-facebook</t>
-  </si>
-  <si>
     <t>Un sistema de posicionamiento impulsa la futura innovación inalámbrica</t>
   </si>
   <si>
@@ -438,55 +441,7 @@
     <t>Socrates project</t>
   </si>
   <si>
-    <t>dasd</t>
-  </si>
-  <si>
-    <t>Number of Posts</t>
-  </si>
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>Classification</t>
-  </si>
-  <si>
-    <t>Source URL</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Twitter</t>
-  </si>
-  <si>
-    <t>@IMDEA_Networks</t>
-  </si>
-  <si>
-    <t>MIT-SPAIN - "la Caixa" Foundation SEED FUND goes to @medialab @IMDEA_Networks @UC3M researchers to conduct research on the influence of user filters in the online #advertising ecosystem http://bit.ly/2CckNeU  @MIT @FundlaCaixa</t>
-  </si>
-  <si>
-    <t>Collaboration</t>
-  </si>
-  <si>
-    <t>https://www.networks.imdea.org/research/projects/mybubble-influence-algorithms-users-filter-bubbles</t>
-  </si>
-  <si>
-    <t>Instagram</t>
-  </si>
-  <si>
-    <t>@imdea_networks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ralf Steinmetz, @IMDEA_Networks Board of Trustees Vice-President, appointed first ITG-Fellow by @VDE_Group, the German Association for Electrical, Electronic &amp; Information Technologies http://bit.ly/2lTft5S </t>
-  </si>
-  <si>
-    <t>Careers</t>
-  </si>
-  <si>
-    <t>https://www.networks.imdea.org/whats-new/news/2017/ralf-steinmetz-appointed-first-itg-fellow-vde-german-association-electrical</t>
+    <t>https://www.esleondiario.com/2018/11/07/como-detectar-y-detener-a-los-saboteadores-del-espectro/</t>
   </si>
   <si>
     <t>Lead Paragraph</t>
@@ -1090,7 +1045,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>43103.04166666667</v>
+        <v>43103</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -1099,16 +1054,16 @@
         <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
@@ -1135,7 +1090,7 @@
         <v>32</v>
       </c>
       <c r="Q3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R3" t="b">
         <v>1</v>
@@ -1150,7 +1105,7 @@
         <v>35</v>
       </c>
       <c r="V3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="W3" t="b">
         <v>0</v>
@@ -1161,25 +1116,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>43103.04166666667</v>
+        <v>43103</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
         <v>29</v>
@@ -1206,7 +1161,7 @@
         <v>32</v>
       </c>
       <c r="Q4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R4" t="b">
         <v>1</v>
@@ -1232,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>43117.04166666667</v>
+        <v>43117</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
@@ -1244,13 +1199,13 @@
         <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
         <v>29</v>
@@ -1274,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="Q5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R5" t="b">
         <v>1</v>
@@ -1300,7 +1255,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2">
-        <v>43158.04166666667</v>
+        <v>43158</v>
       </c>
       <c r="C6" t="s">
         <v>51</v>
@@ -1318,16 +1273,16 @@
         <v>27</v>
       </c>
       <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
         <v>53</v>
-      </c>
-      <c r="I6" t="s">
-        <v>54</v>
       </c>
       <c r="J6" t="s">
         <v>30</v>
       </c>
       <c r="K6" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="L6" t="b">
         <v>0</v>
@@ -1341,8 +1296,11 @@
       <c r="O6" t="b">
         <v>1</v>
       </c>
+      <c r="P6" t="s">
+        <v>54</v>
+      </c>
       <c r="Q6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R6" t="b">
         <v>1</v>
@@ -1368,7 +1326,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>43158.04166666667</v>
+        <v>43158</v>
       </c>
       <c r="C7" t="s">
         <v>57</v>
@@ -1386,16 +1344,16 @@
         <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
         <v>30</v>
       </c>
       <c r="K7" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="L7" t="b">
         <v>0</v>
@@ -1409,11 +1367,8 @@
       <c r="O7" t="b">
         <v>1</v>
       </c>
-      <c r="P7" t="s">
-        <v>60</v>
-      </c>
       <c r="Q7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R7" t="b">
         <v>1</v>
@@ -1439,7 +1394,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2">
-        <v>43169.04166666667</v>
+        <v>43169</v>
       </c>
       <c r="C8" t="s">
         <v>62</v>
@@ -1481,10 +1436,10 @@
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="Q8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R8" t="b">
         <v>1</v>
@@ -1510,7 +1465,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="2">
-        <v>43170.04166666667</v>
+        <v>43170</v>
       </c>
       <c r="C9" t="s">
         <v>68</v>
@@ -1528,7 +1483,7 @@
         <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I9" t="s">
         <v>70</v>
@@ -1552,10 +1507,10 @@
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="Q9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R9" t="b">
         <v>1</v>
@@ -1581,7 +1536,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="2">
-        <v>43171</v>
+        <v>43170.95833333333</v>
       </c>
       <c r="C10" t="s">
         <v>72</v>
@@ -1623,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="P10" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="Q10" t="s">
         <v>33</v>
@@ -1638,10 +1593,10 @@
         <v>65</v>
       </c>
       <c r="U10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="W10" t="b">
         <v>0</v>
@@ -1652,13 +1607,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="2">
-        <v>43171.04166666667</v>
+        <v>43171</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
@@ -1673,7 +1628,7 @@
         <v>31</v>
       </c>
       <c r="I11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J11" t="s">
         <v>30</v>
@@ -1694,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="Q11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R11" t="b">
         <v>1</v>
@@ -1706,10 +1661,10 @@
         <v>65</v>
       </c>
       <c r="U11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="W11" t="b">
         <v>0</v>
@@ -1720,13 +1675,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="2">
-        <v>43173.04166666667</v>
+        <v>43173</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
@@ -1738,10 +1693,10 @@
         <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J12" t="s">
         <v>30</v>
@@ -1762,10 +1717,10 @@
         <v>1</v>
       </c>
       <c r="P12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="Q12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R12" t="b">
         <v>1</v>
@@ -1777,10 +1732,10 @@
         <v>65</v>
       </c>
       <c r="U12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="W12" t="b">
         <v>0</v>
@@ -1791,13 +1746,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="2">
-        <v>43175.04166666667</v>
+        <v>43175</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -1812,7 +1767,7 @@
         <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
         <v>30</v>
@@ -1833,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="Q13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R13" t="b">
         <v>1</v>
@@ -1845,10 +1800,10 @@
         <v>65</v>
       </c>
       <c r="U13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="W13" t="b">
         <v>0</v>
@@ -1859,13 +1814,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="2">
-        <v>43210.08333333333</v>
+        <v>43210</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
@@ -1880,7 +1835,7 @@
         <v>31</v>
       </c>
       <c r="I14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J14" t="s">
         <v>30</v>
@@ -1901,10 +1856,10 @@
         <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R14" t="b">
         <v>1</v>
@@ -1916,10 +1871,10 @@
         <v>34</v>
       </c>
       <c r="U14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="V14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="W14" t="b">
         <v>0</v>
@@ -1930,7 +1885,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="2">
-        <v>43212.08333333333</v>
+        <v>43212</v>
       </c>
       <c r="C15" t="s">
         <v>68</v>
@@ -1948,10 +1903,10 @@
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J15" t="s">
         <v>30</v>
@@ -1972,10 +1927,10 @@
         <v>1</v>
       </c>
       <c r="P15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R15" t="b">
         <v>1</v>
@@ -1987,10 +1942,10 @@
         <v>34</v>
       </c>
       <c r="U15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="V15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="W15" t="b">
         <v>0</v>
@@ -2001,19 +1956,19 @@
         <v>4</v>
       </c>
       <c r="B16" s="2">
-        <v>43213.08333333333</v>
+        <v>43213</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
         <v>27</v>
@@ -2022,7 +1977,7 @@
         <v>31</v>
       </c>
       <c r="I16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J16" t="s">
         <v>30</v>
@@ -2043,10 +1998,10 @@
         <v>1</v>
       </c>
       <c r="P16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R16" t="b">
         <v>1</v>
@@ -2058,10 +2013,10 @@
         <v>34</v>
       </c>
       <c r="U16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="V16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="W16" t="b">
         <v>0</v>
@@ -2072,13 +2027,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="2">
-        <v>43215.08333333333</v>
+        <v>43215</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
@@ -2090,10 +2045,10 @@
         <v>27</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J17" t="s">
         <v>30</v>
@@ -2114,7 +2069,7 @@
         <v>1</v>
       </c>
       <c r="Q17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R17" t="b">
         <v>1</v>
@@ -2126,10 +2081,10 @@
         <v>34</v>
       </c>
       <c r="U17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="V17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W17" t="b">
         <v>0</v>
@@ -2140,13 +2095,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="2">
-        <v>43224</v>
+        <v>43223.91666666667</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
@@ -2158,10 +2113,10 @@
         <v>27</v>
       </c>
       <c r="H18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J18" t="s">
         <v>30</v>
@@ -2182,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="P18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q18" t="s">
         <v>33</v>
@@ -2197,10 +2152,10 @@
         <v>34</v>
       </c>
       <c r="U18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="V18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="W18" t="b">
         <v>0</v>
@@ -2211,13 +2166,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="2">
-        <v>43250</v>
+        <v>43249.91666666667</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
@@ -2232,7 +2187,7 @@
         <v>28</v>
       </c>
       <c r="I19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J19" t="s">
         <v>30</v>
@@ -2253,10 +2208,10 @@
         <v>1</v>
       </c>
       <c r="P19" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="Q19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R19" t="b">
         <v>1</v>
@@ -2268,10 +2223,10 @@
         <v>34</v>
       </c>
       <c r="U19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="W19" t="b">
         <v>0</v>
@@ -2282,13 +2237,13 @@
         <v>6</v>
       </c>
       <c r="B20" s="2">
-        <v>43252.08333333333</v>
+        <v>43252</v>
       </c>
       <c r="C20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
@@ -2300,10 +2255,10 @@
         <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J20" t="s">
         <v>30</v>
@@ -2324,10 +2279,10 @@
         <v>1</v>
       </c>
       <c r="P20" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="Q20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R20" t="b">
         <v>1</v>
@@ -2339,10 +2294,10 @@
         <v>34</v>
       </c>
       <c r="U20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="W20" t="b">
         <v>0</v>
@@ -2353,13 +2308,13 @@
         <v>6</v>
       </c>
       <c r="B21" s="2">
-        <v>43271.08333333333</v>
+        <v>43271</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
@@ -2371,10 +2326,10 @@
         <v>27</v>
       </c>
       <c r="H21" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J21" t="s">
         <v>30</v>
@@ -2394,8 +2349,11 @@
       <c r="O21" t="b">
         <v>1</v>
       </c>
+      <c r="P21" t="s">
+        <v>117</v>
+      </c>
       <c r="Q21" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="R21" t="b">
         <v>1</v>
@@ -2407,10 +2365,10 @@
         <v>65</v>
       </c>
       <c r="U21" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="V21" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="W21" t="b">
         <v>0</v>
@@ -2421,13 +2379,13 @@
         <v>6</v>
       </c>
       <c r="B22" s="2">
-        <v>43271.08333333333</v>
+        <v>43271</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
@@ -2439,10 +2397,10 @@
         <v>27</v>
       </c>
       <c r="H22" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I22" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="J22" t="s">
         <v>30</v>
@@ -2462,11 +2420,8 @@
       <c r="O22" t="b">
         <v>1</v>
       </c>
-      <c r="P22" t="s">
-        <v>119</v>
-      </c>
       <c r="Q22" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="R22" t="b">
         <v>1</v>
@@ -2478,10 +2433,10 @@
         <v>65</v>
       </c>
       <c r="U22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="V22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="W22" t="b">
         <v>0</v>
@@ -2492,13 +2447,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="2">
-        <v>43271.08333333333</v>
+        <v>43271</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="E23" t="s">
         <v>25</v>
@@ -2510,10 +2465,10 @@
         <v>27</v>
       </c>
       <c r="H23" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="I23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J23" t="s">
         <v>30</v>
@@ -2534,10 +2489,10 @@
         <v>1</v>
       </c>
       <c r="P23" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="Q23" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="R23" t="b">
         <v>1</v>
@@ -2549,10 +2504,10 @@
         <v>65</v>
       </c>
       <c r="U23" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="V23" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="W23" t="b">
         <v>0</v>
@@ -2563,13 +2518,13 @@
         <v>6</v>
       </c>
       <c r="B24" s="2">
-        <v>43271.08333333333</v>
+        <v>43271</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
         <v>25</v>
@@ -2581,10 +2536,10 @@
         <v>27</v>
       </c>
       <c r="H24" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="I24" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="J24" t="s">
         <v>30</v>
@@ -2605,10 +2560,10 @@
         <v>1</v>
       </c>
       <c r="P24" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="Q24" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="R24" t="b">
         <v>1</v>
@@ -2620,10 +2575,10 @@
         <v>65</v>
       </c>
       <c r="U24" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="V24" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="W24" t="b">
         <v>0</v>
@@ -2634,13 +2589,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="2">
-        <v>43271.08333333333</v>
+        <v>43271</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E25" t="s">
         <v>25</v>
@@ -2652,10 +2607,10 @@
         <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I25" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J25" t="s">
         <v>30</v>
@@ -2676,10 +2631,10 @@
         <v>1</v>
       </c>
       <c r="P25" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="Q25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R25" t="b">
         <v>1</v>
@@ -2691,10 +2646,10 @@
         <v>65</v>
       </c>
       <c r="U25" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="V25" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="W25" t="b">
         <v>0</v>
@@ -2705,13 +2660,13 @@
         <v>9</v>
       </c>
       <c r="B26" s="2">
-        <v>43347.08333333333</v>
+        <v>43347</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E26" t="s">
         <v>25</v>
@@ -2726,7 +2681,7 @@
         <v>31</v>
       </c>
       <c r="I26" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J26" t="s">
         <v>30</v>
@@ -2747,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="Q26" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R26" t="b">
         <v>1</v>
@@ -2759,10 +2714,10 @@
         <v>65</v>
       </c>
       <c r="U26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="W26" t="b">
         <v>0</v>
@@ -2773,13 +2728,13 @@
         <v>11</v>
       </c>
       <c r="B27" s="2">
-        <v>43411</v>
+        <v>43410.95833333333</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
@@ -2788,13 +2743,13 @@
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H27" t="s">
         <v>28</v>
       </c>
       <c r="I27" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J27" t="s">
         <v>30</v>
@@ -2815,10 +2770,10 @@
         <v>1</v>
       </c>
       <c r="P27" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="Q27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R27" t="b">
         <v>1</v>
@@ -2830,10 +2785,10 @@
         <v>34</v>
       </c>
       <c r="U27" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V27" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="W27" t="b">
         <v>0</v>
@@ -2848,143 +2803,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:A1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43678</v>
-      </c>
-      <c r="D2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" t="s">
-        <v>151</v>
-      </c>
-      <c r="L2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M2" t="s">
-        <v>152</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2">
-        <v>43684</v>
-      </c>
-      <c r="D3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" t="s">
-        <v>156</v>
-      </c>
-      <c r="L3" t="s">
-        <v>133</v>
-      </c>
-      <c r="M3" t="s">
-        <v>157</v>
-      </c>
-      <c r="N3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:V1"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
@@ -3009,16 +2830,16 @@
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3026,22 +2847,22 @@
         <v>12</v>
       </c>
       <c r="B2" s="2">
-        <v>43098.04166666667</v>
+        <v>43098</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F2" t="s">
         <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -3052,22 +2873,22 @@
         <v>12</v>
       </c>
       <c r="B3" s="2">
-        <v>43098.04166666667</v>
+        <v>43098</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
         <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -3078,22 +2899,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>43165.04166666667</v>
+        <v>43165</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
         <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F4" t="s">
         <v>65</v>
       </c>
       <c r="G4" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -3104,22 +2925,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>43172.04166666667</v>
+        <v>43172</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F5" t="s">
         <v>65</v>
       </c>
       <c r="G5" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -3130,22 +2951,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>43209.08333333333</v>
+        <v>43209</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -3156,22 +2977,22 @@
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>43214.08333333333</v>
+        <v>43214</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -3182,22 +3003,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>43231.08333333333</v>
+        <v>43231</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E8" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F8" t="s">
         <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -3208,22 +3029,22 @@
         <v>5</v>
       </c>
       <c r="B9" s="2">
-        <v>43250.08333333333</v>
+        <v>43250</v>
       </c>
       <c r="C9" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E9" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F9" t="s">
         <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -3234,22 +3055,22 @@
         <v>6</v>
       </c>
       <c r="B10" s="2">
-        <v>43271.08333333333</v>
+        <v>43271</v>
       </c>
       <c r="C10" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F10" t="s">
         <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -3260,22 +3081,22 @@
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>43343.08333333333</v>
+        <v>43343</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F11" t="s">
         <v>65</v>
       </c>
       <c r="G11" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>

</xml_diff>